<commit_message>
Dynamic excel reader @DataProvider
</commit_message>
<xml_diff>
--- a/ExcelReader/testData/DataSheet.xlsx
+++ b/ExcelReader/testData/DataSheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5F11940E-E28B-4E26-88E8-BABDBB8E773E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F0DDEA5D-3D34-4E40-A9F7-F0DA9689CFB4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,22 +53,22 @@
     <t>TestCase1</t>
   </si>
   <si>
-    <t>02_NormalEstabEntryPermitTourism</t>
-  </si>
-  <si>
     <t>TestCase2</t>
   </si>
   <si>
-    <t>03_NormalEstabEntryPermitTourism</t>
-  </si>
-  <si>
-    <t>04_NormalEstabEntryPermitTourism</t>
-  </si>
-  <si>
     <t>TestCase3</t>
   </si>
   <si>
     <t>TestCase4</t>
+  </si>
+  <si>
+    <t>02_Normal</t>
+  </si>
+  <si>
+    <t>03_EstabEntry</t>
+  </si>
+  <si>
+    <t>04_Tourism</t>
   </si>
 </sst>
 </file>
@@ -423,7 +423,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -450,26 +450,26 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Handling null values while reading from Excel sheet
</commit_message>
<xml_diff>
--- a/ExcelReader/testData/DataSheet.xlsx
+++ b/ExcelReader/testData/DataSheet.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F0DDEA5D-3D34-4E40-A9F7-F0DA9689CFB4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100800_{1CFF0DA1-2071-426E-92C5-680F39A20649}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14150" windowHeight="5590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
     <sheet name="TestConfig" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -51,9 +52,6 @@
   </si>
   <si>
     <t>TestCase1</t>
-  </si>
-  <si>
-    <t>TestCase2</t>
   </si>
   <si>
     <t>TestCase3</t>
@@ -423,7 +421,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -450,26 +448,24 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Retrieve row from table using test case name [or any row value you can configure].
</commit_message>
<xml_diff>
--- a/ExcelReader/testData/DataSheet.xlsx
+++ b/ExcelReader/testData/DataSheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100800_{1CFF0DA1-2071-426E-92C5-680F39A20649}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100800_{88697896-CF6F-4631-8D9A-19A1DF00B276}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14150" windowHeight="5590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,9 +48,6 @@
     <t>qovnv74n1</t>
   </si>
   <si>
-    <t>01_EstabLogin</t>
-  </si>
-  <si>
     <t>TestCase1</t>
   </si>
   <si>
@@ -60,13 +57,16 @@
     <t>TestCase4</t>
   </si>
   <si>
-    <t>02_Normal</t>
-  </si>
-  <si>
-    <t>03_EstabEntry</t>
-  </si>
-  <si>
-    <t>04_Tourism</t>
+    <t>T01_EstabLogin</t>
+  </si>
+  <si>
+    <t>T02_Normal</t>
+  </si>
+  <si>
+    <t>T03_EstabEntry</t>
+  </si>
+  <si>
+    <t>T04_Tourism</t>
   </si>
 </sst>
 </file>
@@ -421,7 +421,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -440,10 +440,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -457,7 +457,7 @@
         <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -465,7 +465,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>